<commit_message>
wow this is not going quickly at all
</commit_message>
<xml_diff>
--- a/ML10data.xlsx
+++ b/ML10data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williamshue/Downloads/naive-bayes-classifier/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDE13283-ACDB-0A42-9039-B8661D7EA650}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA39CD3-4D56-1940-BFFB-0FC0CF36F58F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2240" yWindow="460" windowWidth="23260" windowHeight="17540" xr2:uid="{EFA67FC4-7DAC-4450-8E12-5B45F1787297}"/>
   </bookViews>
@@ -1257,7 +1257,7 @@
   <dimension ref="E2:N49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>